<commit_message>
+session; add instrument user-count to json sheet
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="store" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ready_to_sale" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Лист4" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sales" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sales Ua" sheetId="4" state="visible" r:id="rId5"/>
@@ -267,30 +267,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="106">
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Инструменты г</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">отовые к отправке</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="109">
+  <si>
+    <t xml:space="preserve">Инструменты</t>
   </si>
   <si>
     <r>
@@ -332,46 +311,55 @@
     <t xml:space="preserve">Waterfall</t>
   </si>
   <si>
+    <t xml:space="preserve">Ether-Acril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ether-Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infinity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eternal-love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комплектация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Не упакованы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bag стандарт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bag эфир</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Box Divya</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ether Acril </t>
   </si>
   <si>
+    <t xml:space="preserve">Планки дерево Б</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ether Wood</t>
   </si>
   <si>
-    <t xml:space="preserve">Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infinity</t>
+    <t xml:space="preserve">Планки дерево М</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Планки акрил Б</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Планки  акрил М</t>
   </si>
   <si>
     <t xml:space="preserve">Eternal love</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Комплектация</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Не упакованы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bag стандарт</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bag эфир</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Box Divya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Планки дерево Б</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Планки дерево М</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Планки акрил Б</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Планки  акрил М</t>
   </si>
   <si>
     <t xml:space="preserve">Подставки </t>
@@ -1031,17 +1019,17 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.53"/>
   </cols>
   <sheetData>
@@ -1297,9 +1285,9 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.01"/>
   </cols>
   <sheetData>
@@ -1351,28 +1339,28 @@
       </c>
       <c r="C4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="15" t="n">
         <v>12</v>
       </c>
       <c r="C5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="15" t="n">
         <v>10</v>
@@ -1386,7 +1374,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="7"/>
@@ -1400,19 +1388,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" s="15" t="n">
         <v>6</v>
@@ -1421,14 +1409,14 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>50</v>
@@ -1458,7 +1446,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.63"/>
@@ -1467,34 +1455,34 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1545,20 +1533,20 @@
         <v>10</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,20 +1561,20 @@
         <v>9</v>
       </c>
       <c r="E7" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>36</v>
-      </c>
       <c r="H7" s="22" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,20 +1589,20 @@
         <v>6</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,23 +1614,23 @@
         <v>360</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1659,13 +1647,13 @@
         <v>5</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
@@ -1685,22 +1673,22 @@
         <v>10</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1715,22 +1703,22 @@
         <v>5</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,25 +1732,25 @@
         <v>360</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,18 +1767,18 @@
         <v>6</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,22 +1795,22 @@
         <v>5</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,23 +1824,23 @@
         <v>160</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I16" s="18"/>
       <c r="J16" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,18 +1857,18 @@
         <v>5</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,18 +1881,18 @@
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,21 +1906,21 @@
         <v>87</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I19" s="18"/>
       <c r="J19" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,17 +1934,17 @@
         <v>216</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
@@ -1975,10 +1963,10 @@
         <v>9</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="29"/>
@@ -2019,7 +2007,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.63"/>
@@ -2029,25 +2017,25 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,17 +2055,17 @@
         <v>5000</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,14 +2076,14 @@
         <v>5500</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G5" s="18"/>
     </row>
@@ -2111,13 +2099,13 @@
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2128,17 +2116,17 @@
         <v>5500</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>91</v>
-      </c>
       <c r="G7" s="18" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,17 +2137,17 @@
         <v>5500</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2174,10 +2162,10 @@
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G9" s="18"/>
     </row>
@@ -2189,17 +2177,17 @@
         <v>5500</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,13 +2202,13 @@
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,10 +2223,10 @@
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G12" s="18"/>
     </row>
@@ -2254,10 +2242,10 @@
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G13" s="18"/>
     </row>
@@ -2273,10 +2261,10 @@
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G14" s="18"/>
     </row>
@@ -2288,14 +2276,14 @@
         <v>4500</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G15" s="18"/>
     </row>
@@ -2313,7 +2301,7 @@
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2318,7 @@
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,11 +2329,11 @@
         <v>3000</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
@@ -2358,11 +2346,11 @@
         <v>4200</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="22" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -2379,7 +2367,7 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,7 +2382,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
some minor fix; add instrument to sheet++
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -726,14 +726,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFF9F9F9"/>
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFC9DAF8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCFE2F3"/>
-        <bgColor rgb="FFC9DAF8"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF9F9F9"/>
       </patternFill>
     </fill>
     <fill>
@@ -743,7 +743,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -765,21 +765,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -806,7 +791,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -859,10 +844,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -871,11 +852,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -887,7 +868,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -895,7 +876,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -903,7 +884,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -911,11 +892,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -923,7 +904,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -964,7 +945,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1016,13 +997,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1048576"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.92"/>
@@ -1185,16 +1166,9 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="13"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-    </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="6"/>
@@ -1232,36 +1206,12 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1285,19 +1235,19 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="7"/>
@@ -1306,7 +1256,7 @@
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="15" t="n">
+      <c r="B2" s="14" t="n">
         <v>20</v>
       </c>
       <c r="C2" s="7"/>
@@ -1320,7 +1270,7 @@
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="15" t="n">
+      <c r="B3" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C3" s="7"/>
@@ -1334,7 +1284,7 @@
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="15" t="n">
+      <c r="B4" s="14" t="n">
         <v>43</v>
       </c>
       <c r="C4" s="7"/>
@@ -1348,7 +1298,7 @@
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15" t="n">
+      <c r="B5" s="14" t="n">
         <v>12</v>
       </c>
       <c r="C5" s="7"/>
@@ -1362,7 +1312,7 @@
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="15" t="n">
+      <c r="B6" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C6" s="7"/>
@@ -1376,13 +1326,13 @@
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="7"/>
       <c r="E7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="15" t="n">
+      <c r="G7" s="14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1390,7 +1340,7 @@
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="7"/>
       <c r="E8" s="7" t="s">
         <v>23</v>
@@ -1402,7 +1352,7 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="15" t="n">
+      <c r="B9" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="7"/>
@@ -1446,7 +1396,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.63"/>
@@ -1454,536 +1404,536 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="n">
+      <c r="A6" s="19" t="n">
         <v>44790</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="21" t="n">
+      <c r="B6" s="18"/>
+      <c r="C6" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="17"/>
+      <c r="J6" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="n">
+      <c r="A7" s="19" t="n">
         <v>44789</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="21" t="n">
+      <c r="B7" s="18"/>
+      <c r="C7" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="22" t="s">
+      <c r="I7" s="17"/>
+      <c r="J7" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="n">
+      <c r="A8" s="19" t="n">
         <v>44789</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="21" t="n">
+      <c r="B8" s="18"/>
+      <c r="C8" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="22" t="s">
+      <c r="I8" s="17"/>
+      <c r="J8" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="n">
+      <c r="A9" s="19" t="n">
         <v>44782</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="21" t="n">
+      <c r="B9" s="18"/>
+      <c r="C9" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="22" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="n">
+      <c r="A10" s="24" t="n">
         <v>44776</v>
       </c>
-      <c r="B10" s="26" t="n">
+      <c r="B10" s="25" t="n">
         <v>44784</v>
       </c>
-      <c r="C10" s="21" t="n">
+      <c r="C10" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="n">
+      <c r="A11" s="24" t="n">
         <v>44776</v>
       </c>
-      <c r="B11" s="26" t="n">
+      <c r="B11" s="25" t="n">
         <v>44784</v>
       </c>
-      <c r="C11" s="21" t="n">
+      <c r="C11" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="n">
+      <c r="A12" s="24" t="n">
         <v>44776</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="21" t="n">
+      <c r="B12" s="18"/>
+      <c r="C12" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="n">
+      <c r="A13" s="19" t="n">
         <v>44769</v>
       </c>
-      <c r="B13" s="19" t="n">
+      <c r="B13" s="18" t="n">
         <v>44777</v>
       </c>
-      <c r="C13" s="21" t="n">
+      <c r="C13" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="n">
+      <c r="A14" s="19" t="n">
         <v>44769</v>
       </c>
-      <c r="B14" s="19" t="n">
+      <c r="B14" s="18" t="n">
         <v>44777</v>
       </c>
-      <c r="C14" s="21" t="n">
+      <c r="C14" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="22" t="s">
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="n">
+      <c r="A15" s="19" t="n">
         <v>44769</v>
       </c>
-      <c r="B15" s="19" t="n">
+      <c r="B15" s="18" t="n">
         <v>44777</v>
       </c>
-      <c r="C15" s="21" t="n">
+      <c r="C15" s="20" t="n">
         <v>360</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27" t="n">
+      <c r="A16" s="26" t="n">
         <v>44758</v>
       </c>
-      <c r="B16" s="26" t="n">
+      <c r="B16" s="25" t="n">
         <v>44784</v>
       </c>
-      <c r="C16" s="21" t="n">
+      <c r="C16" s="20" t="n">
         <v>160</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18" t="s">
+      <c r="I16" s="17"/>
+      <c r="J16" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="n">
+      <c r="A17" s="24" t="n">
         <v>44753</v>
       </c>
-      <c r="B17" s="26" t="n">
+      <c r="B17" s="25" t="n">
         <v>44767</v>
       </c>
-      <c r="C17" s="18" t="n">
+      <c r="C17" s="17" t="n">
         <v>360</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18" t="s">
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25" t="n">
+      <c r="A18" s="24" t="n">
         <v>44743</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="28" t="n">
+      <c r="B18" s="18"/>
+      <c r="C18" s="27" t="n">
         <v>240</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18" t="s">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18" t="s">
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="25" t="n">
+      <c r="A19" s="24" t="n">
         <v>44743</v>
       </c>
-      <c r="B19" s="19" t="n">
+      <c r="B19" s="18" t="n">
         <v>44777</v>
       </c>
-      <c r="C19" s="28" t="n">
+      <c r="C19" s="27" t="n">
         <v>87</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="22" t="s">
+      <c r="G19" s="17"/>
+      <c r="H19" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18" t="s">
+      <c r="I19" s="17"/>
+      <c r="J19" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25" t="n">
+      <c r="A20" s="24" t="n">
         <v>44743</v>
       </c>
-      <c r="B20" s="19" t="n">
+      <c r="B20" s="18" t="n">
         <v>44777</v>
       </c>
-      <c r="C20" s="28" t="n">
+      <c r="C20" s="27" t="n">
         <v>216</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="24" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="25" t="n">
+      <c r="A21" s="24" t="n">
         <v>44743</v>
       </c>
-      <c r="B21" s="19" t="n">
+      <c r="B21" s="18" t="n">
         <v>44777</v>
       </c>
-      <c r="C21" s="28" t="n">
+      <c r="C21" s="27" t="n">
         <v>216</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2007,7 +1957,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.63"/>
@@ -2016,383 +1966,383 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="31" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="n">
+      <c r="A4" s="24" t="n">
         <v>44789</v>
       </c>
-      <c r="B4" s="18" t="n">
+      <c r="B4" s="17" t="n">
         <v>5000</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="n">
+      <c r="A5" s="24" t="n">
         <v>44789</v>
       </c>
-      <c r="B5" s="18" t="n">
+      <c r="B5" s="17" t="n">
         <v>5500</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="n">
+      <c r="A6" s="24" t="n">
         <v>44789</v>
       </c>
-      <c r="B6" s="18" t="n">
+      <c r="B6" s="17" t="n">
         <v>5250</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="n">
+      <c r="A7" s="24" t="n">
         <v>44788</v>
       </c>
-      <c r="B7" s="18" t="n">
+      <c r="B7" s="17" t="n">
         <v>5500</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="n">
+      <c r="A8" s="24" t="n">
         <v>44785</v>
       </c>
-      <c r="B8" s="18" t="n">
+      <c r="B8" s="17" t="n">
         <v>5500</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="n">
+      <c r="A9" s="24" t="n">
         <v>44775</v>
       </c>
-      <c r="B9" s="18" t="n">
+      <c r="B9" s="17" t="n">
         <v>4500</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="n">
+      <c r="A10" s="24" t="n">
         <v>44780</v>
       </c>
-      <c r="B10" s="18" t="n">
+      <c r="B10" s="17" t="n">
         <v>5500</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18" t="s">
+      <c r="D10" s="17"/>
+      <c r="E10" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="n">
+      <c r="A11" s="24" t="n">
         <v>44771</v>
       </c>
-      <c r="B11" s="18" t="n">
+      <c r="B11" s="17" t="n">
         <v>5500</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="n">
+      <c r="A12" s="24" t="n">
         <v>44771</v>
       </c>
-      <c r="B12" s="18" t="n">
+      <c r="B12" s="17" t="n">
         <v>4500</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="n">
+      <c r="A13" s="24" t="n">
         <v>44771</v>
       </c>
-      <c r="B13" s="18" t="n">
+      <c r="B13" s="17" t="n">
         <v>4500</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="18"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="n">
+      <c r="A14" s="24" t="n">
         <v>44771</v>
       </c>
-      <c r="B14" s="18" t="n">
+      <c r="B14" s="17" t="n">
         <v>4500</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18" t="s">
+      <c r="D14" s="17"/>
+      <c r="E14" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="18"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="n">
+      <c r="A15" s="24" t="n">
         <v>44771</v>
       </c>
-      <c r="B15" s="18" t="n">
+      <c r="B15" s="17" t="n">
         <v>4500</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="17"/>
+      <c r="E15" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="n">
+      <c r="A16" s="24" t="n">
         <v>44766</v>
       </c>
-      <c r="B16" s="18" t="n">
+      <c r="B16" s="17" t="n">
         <v>4675</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18" t="s">
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="n">
+      <c r="A17" s="24" t="n">
         <v>44766</v>
       </c>
-      <c r="B17" s="18" t="n">
+      <c r="B17" s="17" t="n">
         <v>4675</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18" t="s">
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25" t="n">
+      <c r="A18" s="24" t="n">
         <v>44766</v>
       </c>
-      <c r="B18" s="18" t="n">
+      <c r="B18" s="17" t="n">
         <v>3000</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18" t="s">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="25" t="n">
+      <c r="A19" s="24" t="n">
         <v>44766</v>
       </c>
-      <c r="B19" s="18" t="n">
+      <c r="B19" s="17" t="n">
         <v>4200</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="22" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25" t="n">
+      <c r="A20" s="24" t="n">
         <v>44756</v>
       </c>
-      <c r="B20" s="18" t="n">
+      <c r="B20" s="17" t="n">
         <v>4775</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18" t="s">
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="25" t="n">
+      <c r="A21" s="24" t="n">
         <v>44756</v>
       </c>
-      <c r="B21" s="18" t="n">
+      <c r="B21" s="17" t="n">
         <v>4775</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
write to table writeOff materials
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -517,10 +517,10 @@
         <v>Fire</v>
       </c>
       <c r="B2" s="1">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -660,7 +660,7 @@
         <v>Bag стандарт</v>
       </c>
       <c r="B2" s="1">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -684,7 +684,7 @@
         <v>Планки дерево Б</v>
       </c>
       <c r="B5" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -692,7 +692,7 @@
         <v>Планки дерево М</v>
       </c>
       <c r="B6" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -716,7 +716,7 @@
         <v>Подставки</v>
       </c>
       <c r="B9" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -732,7 +732,7 @@
         <v>Стики</v>
       </c>
       <c r="B11" s="1">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add session states obj
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -433,7 +433,7 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D2" t="str">
         <v>1</v>
@@ -570,8 +570,8 @@
       <c r="A2" t="str">
         <v>Bag стандарт</v>
       </c>
-      <c r="B2" t="str">
-        <v>50</v>
+      <c r="B2">
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -594,16 +594,16 @@
       <c r="A5" t="str">
         <v>Планки дерево Б</v>
       </c>
-      <c r="B5" t="str">
-        <v>50</v>
+      <c r="B5">
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Планки дерево М</v>
       </c>
-      <c r="B6" t="str">
-        <v>50</v>
+      <c r="B6">
+        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -626,8 +626,8 @@
       <c r="A9" t="str">
         <v>Подставки</v>
       </c>
-      <c r="B9" t="str">
-        <v>50</v>
+      <c r="B9">
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -643,7 +643,7 @@
         <v>Стики</v>
       </c>
       <c r="B11">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
writeOff box for ENG
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -4,9 +4,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <sheets>
     <sheet name="ready_to_sale" sheetId="1" r:id="rId1"/>
-    <sheet name="components" sheetId="2" r:id="rId2"/>
-    <sheet name="Sales" sheetId="3" r:id="rId3"/>
-    <sheet name="Sales Ua" sheetId="4" r:id="rId4"/>
+    <sheet name="tubes" sheetId="2" r:id="rId2"/>
+    <sheet name="components" sheetId="3" r:id="rId3"/>
+    <sheet name="Sales" sheetId="4" r:id="rId4"/>
+    <sheet name="Sales Ua" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -430,10 +431,10 @@
         <v>Fire</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -447,7 +448,7 @@
         <v>Waterfall</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -498,10 +499,10 @@
         <v>Alchemy</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -515,10 +516,10 @@
         <v>Infinity</v>
       </c>
       <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
         <v>3</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -554,7 +555,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A2:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Fire</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Waterfall</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Ether-Acril</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Ether-Wood</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Alchemy</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Infinity</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Eternal-love</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A2:A8"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -572,7 +623,7 @@
         <v>Bag стандарт</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -588,7 +639,7 @@
         <v>Box Divya</v>
       </c>
       <c r="B4">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5">
@@ -596,7 +647,7 @@
         <v>Планки дерево Б</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -604,7 +655,7 @@
         <v>Планки дерево М</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -628,7 +679,7 @@
         <v>Подставки</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -644,7 +695,7 @@
         <v>Стики</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
@@ -660,7 +711,7 @@
         <v>Флизелин Ефир</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -684,7 +735,7 @@
         <v>Миникорд 110 см</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -711,31 +762,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Пенка 130 см</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>Пенка 250 см</v>
-      </c>
-      <c r="B21">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B19"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:J21"/>
   <sheetViews>
@@ -756,26 +791,26 @@
         <v>Описание</v>
       </c>
       <c r="E2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Имя_x000d_
+        <v xml:space="preserve">Имя_x000d__x000d_
 покупателя</v>
       </c>
       <c r="F2" t="str">
         <v>Страна</v>
       </c>
       <c r="G2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Откуда_x000d_
+        <v xml:space="preserve">Откуда_x000d__x000d_
 покупатель</v>
       </c>
       <c r="H2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Track_x000d_
+        <v xml:space="preserve">Track_x000d__x000d_
 number</v>
       </c>
       <c r="I2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Стоимость_x000d_
+        <v xml:space="preserve">Стоимость_x000d__x000d_
 доставки</v>
       </c>
       <c r="J2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Почтовая_x000d_
+        <v xml:space="preserve">Почтовая_x000d__x000d_
 служба</v>
       </c>
     </row>
@@ -1209,7 +1244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G21"/>
   <sheetViews>

</xml_diff>

<commit_message>
add and remove no complect instruments
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="ready_to_sale" sheetId="1" r:id="rId1"/>
     <sheet name="tubes" sheetId="2" r:id="rId2"/>
@@ -405,9 +405,6 @@
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -430,16 +427,16 @@
       <c r="A2" t="str">
         <v>Fire</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="str">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="str">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="str">
         <v>3</v>
       </c>
     </row>
@@ -447,16 +444,16 @@
       <c r="A3" t="str">
         <v>Waterfall</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="str">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="str">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="str">
         <v>4</v>
       </c>
     </row>
@@ -464,16 +461,16 @@
       <c r="A4" t="str">
         <v>Ether-Acril</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="str">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="str">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="str">
         <v>5</v>
       </c>
     </row>
@@ -481,16 +478,16 @@
       <c r="A5" t="str">
         <v>Ether-Wood</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="str">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="str">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="str">
         <v>6</v>
       </c>
     </row>
@@ -498,16 +495,16 @@
       <c r="A6" t="str">
         <v>Alchemy</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="str">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="str">
         <v>6</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="str">
         <v>7</v>
       </c>
     </row>
@@ -515,16 +512,16 @@
       <c r="A7" t="str">
         <v>Infinity</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="str">
         <v>3</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="str">
         <v>7</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="str">
         <v>8</v>
       </c>
     </row>
@@ -532,21 +529,20 @@
       <c r="A8" t="str">
         <v>Eternal-love</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="str">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="str">
         <v>8</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="str">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
   </ignoredErrors>
@@ -555,50 +551,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Инструменты</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Количество</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Комментарий</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Fire</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Waterfall</v>
       </c>
+      <c r="B3" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>Ether-Acril</v>
       </c>
+      <c r="B4" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
         <v>Ether-Wood</v>
       </c>
+      <c r="B5" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Alchemy</v>
       </c>
+      <c r="B6" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>Infinity</v>
       </c>
+      <c r="B7" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>Eternal-love</v>
       </c>
+      <c r="B8" t="str">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A2:A8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -622,7 +649,7 @@
       <c r="A2" t="str">
         <v>Bag стандарт</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
         <v>23</v>
       </c>
     </row>
@@ -630,7 +657,7 @@
       <c r="A3" t="str">
         <v>Bag эфир</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
         <v>45</v>
       </c>
     </row>
@@ -638,7 +665,7 @@
       <c r="A4" t="str">
         <v>Box Divya</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
         <v>106</v>
       </c>
     </row>
@@ -646,7 +673,7 @@
       <c r="A5" t="str">
         <v>Планки дерево Б</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
         <v>23</v>
       </c>
     </row>
@@ -654,7 +681,7 @@
       <c r="A6" t="str">
         <v>Планки дерево М</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
         <v>23</v>
       </c>
     </row>
@@ -662,7 +689,7 @@
       <c r="A7" t="str">
         <v>Планки акрил Б</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
         <v>45</v>
       </c>
     </row>
@@ -670,7 +697,7 @@
       <c r="A8" t="str">
         <v>Планки акрил М</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <v>45</v>
       </c>
     </row>
@@ -678,7 +705,7 @@
       <c r="A9" t="str">
         <v>Подставки</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="str">
         <v>23</v>
       </c>
     </row>
@@ -686,7 +713,7 @@
       <c r="A10" t="str">
         <v>Подставки акрил</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="str">
         <v>45</v>
       </c>
     </row>
@@ -694,7 +721,7 @@
       <c r="A11" t="str">
         <v>Стики</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="str">
         <v>18</v>
       </c>
     </row>
@@ -702,7 +729,7 @@
       <c r="A12" t="str">
         <v>Флизелин стандарт</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="str">
         <v>0</v>
       </c>
     </row>
@@ -710,7 +737,7 @@
       <c r="A13" t="str">
         <v>Флизелин Ефир</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="str">
         <v>10</v>
       </c>
     </row>
@@ -718,7 +745,7 @@
       <c r="A14" t="str">
         <v>Паракорд 35 см</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="str">
         <v>0</v>
       </c>
     </row>
@@ -726,7 +753,7 @@
       <c r="A15" t="str">
         <v>Паракорд 48 см</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="str">
         <v>0</v>
       </c>
     </row>
@@ -734,7 +761,7 @@
       <c r="A16" t="str">
         <v>Миникорд 110 см</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="str">
         <v>0</v>
       </c>
     </row>
@@ -742,7 +769,7 @@
       <c r="A17" t="str">
         <v>Миникорд 170 см</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="str">
         <v>0</v>
       </c>
     </row>
@@ -750,7 +777,7 @@
       <c r="A18" t="str">
         <v>Войлок 85х50 см</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="str">
         <v>0</v>
       </c>
     </row>
@@ -758,12 +785,11 @@
       <c r="A19" t="str">
         <v>Замша 80х50 см</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="str">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:B19"/>
   </ignoredErrors>
@@ -772,60 +798,86 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
+    <row r="1" xml:space="preserve">
+      <c r="A1" t="str">
         <v>Отправка</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B1" t="str">
         <v>Получение</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C1" t="str">
         <v xml:space="preserve">Сумма </v>
       </c>
-      <c r="D2" t="str">
+      <c r="D1" t="str">
         <v>Описание</v>
       </c>
-      <c r="E2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Имя_x000d__x000d_
+      <c r="E1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Имя
 покупателя</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F1" t="str">
         <v>Страна</v>
       </c>
-      <c r="G2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Откуда_x000d__x000d_
+      <c r="G1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Откуда
 покупатель</v>
       </c>
-      <c r="H2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Track_x000d__x000d_
+      <c r="H1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Track
 number</v>
       </c>
-      <c r="I2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Стоимость_x000d__x000d_
+      <c r="I1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Стоимость
 доставки</v>
       </c>
-      <c r="J2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Почтовая_x000d__x000d_
+      <c r="J1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Почтовая
 служба</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>44790</v>
+      </c>
+      <c r="C5" t="str">
+        <v>360</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Infinity</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Vasile Christian</v>
+      </c>
+      <c r="F5" t="str">
+        <v>United States</v>
+      </c>
+      <c r="G5" t="str">
+        <v xml:space="preserve"> Etsy</v>
+      </c>
+      <c r="H5" t="str">
+        <v>1ZA6071R0497715606</v>
+      </c>
+      <c r="J5" t="str">
+        <v>UPS</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>44790</v>
+        <v>44789</v>
       </c>
       <c r="C6" t="str">
         <v>360</v>
       </c>
       <c r="D6" t="str">
-        <v>Infinity</v>
+        <v>Alchemy</v>
       </c>
       <c r="E6" t="str">
-        <v>Vasile Christian</v>
+        <v>WILLIAM M GUAY</v>
       </c>
       <c r="F6" t="str">
         <v>United States</v>
@@ -834,7 +886,7 @@
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H6" t="str">
-        <v>1ZA6071R0497715606</v>
+        <v>1ZA6071R0494460726</v>
       </c>
       <c r="J6" t="str">
         <v>UPS</v>
@@ -848,19 +900,19 @@
         <v>360</v>
       </c>
       <c r="D7" t="str">
-        <v>Alchemy</v>
+        <v>Waterfall</v>
       </c>
       <c r="E7" t="str">
-        <v>WILLIAM M GUAY</v>
+        <v>Yulia Malkin</v>
       </c>
       <c r="F7" t="str">
-        <v>United States</v>
+        <v>Canada</v>
       </c>
       <c r="G7" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H7" t="str">
-        <v>1ZA6071R0494460726</v>
+        <v>1ZA6071R0491898117</v>
       </c>
       <c r="J7" t="str">
         <v>UPS</v>
@@ -868,25 +920,25 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>44789</v>
+        <v>44782</v>
       </c>
       <c r="C8" t="str">
         <v>360</v>
       </c>
       <c r="D8" t="str">
-        <v>Waterfall</v>
+        <v>Ether</v>
       </c>
       <c r="E8" t="str">
-        <v>Yulia Malkin</v>
+        <v>Tom Brouwer</v>
       </c>
       <c r="F8" t="str">
-        <v>Canada</v>
+        <v>Netherlands</v>
       </c>
       <c r="G8" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H8" t="str">
-        <v>1ZA6071R0491898117</v>
+        <v>1ZA6071R0491977602</v>
       </c>
       <c r="J8" t="str">
         <v>UPS</v>
@@ -894,28 +946,25 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>44782</v>
+        <v>44776</v>
+      </c>
+      <c r="B9" t="str">
+        <v>44784</v>
       </c>
       <c r="C9" t="str">
         <v>360</v>
       </c>
       <c r="D9" t="str">
-        <v>Ether</v>
+        <v>Fire</v>
       </c>
       <c r="E9" t="str">
-        <v>Tom Brouwer</v>
+        <v>Paul Chek</v>
       </c>
       <c r="F9" t="str">
-        <v>Netherlands</v>
+        <v>United States</v>
       </c>
       <c r="G9" t="str">
         <v xml:space="preserve"> Etsy</v>
-      </c>
-      <c r="H9" t="str">
-        <v>1ZA6071R0491977602</v>
-      </c>
-      <c r="J9" t="str">
-        <v>UPS</v>
       </c>
     </row>
     <row r="10">
@@ -929,77 +978,86 @@
         <v>360</v>
       </c>
       <c r="D10" t="str">
-        <v>Fire</v>
+        <v>Infinity</v>
       </c>
       <c r="E10" t="str">
-        <v>Paul Chek</v>
+        <v>Stephen Huggins</v>
       </c>
       <c r="F10" t="str">
         <v>United States</v>
       </c>
       <c r="G10" t="str">
         <v xml:space="preserve"> Etsy</v>
+      </c>
+      <c r="H10" t="str">
+        <v>1ZA6071R0493815756</v>
+      </c>
+      <c r="I10" t="str">
+        <v>$ 53.68</v>
+      </c>
+      <c r="J10" t="str">
+        <v>UPS</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
         <v>44776</v>
       </c>
-      <c r="B11" t="str">
-        <v>44784</v>
-      </c>
       <c r="C11" t="str">
         <v>360</v>
       </c>
       <c r="D11" t="str">
-        <v>Infinity</v>
+        <v>Fire</v>
       </c>
       <c r="E11" t="str">
-        <v>Stephen Huggins</v>
+        <v>Veselina Popova</v>
       </c>
       <c r="F11" t="str">
-        <v>United States</v>
+        <v>France</v>
       </c>
       <c r="G11" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H11" t="str">
-        <v>1ZA6071R0493815756</v>
+        <v>RH069864023UA</v>
       </c>
       <c r="I11" t="str">
-        <v>$ 53.68</v>
+        <v>$ 24.75</v>
       </c>
       <c r="J11" t="str">
-        <v>UPS</v>
+        <v>UkrPoshta</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>44776</v>
+        <v>44769</v>
+      </c>
+      <c r="B12" t="str">
+        <v>44777</v>
       </c>
       <c r="C12" t="str">
         <v>360</v>
       </c>
       <c r="D12" t="str">
-        <v>Fire</v>
+        <v>Ether</v>
       </c>
       <c r="E12" t="str">
-        <v>Veselina Popova</v>
+        <v>Fawntice McCain</v>
       </c>
       <c r="F12" t="str">
-        <v>France</v>
+        <v>United States</v>
       </c>
       <c r="G12" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H12" t="str">
-        <v>RH069864023UA</v>
+        <v>1ZA6071R0493130987</v>
       </c>
       <c r="I12" t="str">
-        <v>$ 24.75</v>
+        <v>76.54</v>
       </c>
       <c r="J12" t="str">
-        <v>UkrPoshta</v>
+        <v>UPS</v>
       </c>
     </row>
     <row r="13">
@@ -1013,7 +1071,7 @@
         <v>360</v>
       </c>
       <c r="D13" t="str">
-        <v>Ether</v>
+        <v>Waterfall</v>
       </c>
       <c r="E13" t="str">
         <v>Fawntice McCain</v>
@@ -1023,12 +1081,6 @@
       </c>
       <c r="G13" t="str">
         <v xml:space="preserve"> Etsy</v>
-      </c>
-      <c r="H13" t="str">
-        <v>1ZA6071R0493130987</v>
-      </c>
-      <c r="I13" t="str">
-        <v>76.54</v>
       </c>
       <c r="J13" t="str">
         <v>UPS</v>
@@ -1045,10 +1097,10 @@
         <v>360</v>
       </c>
       <c r="D14" t="str">
-        <v>Waterfall</v>
+        <v>Fire</v>
       </c>
       <c r="E14" t="str">
-        <v>Fawntice McCain</v>
+        <v>Mary Casey Bowers</v>
       </c>
       <c r="F14" t="str">
         <v>United States</v>
@@ -1056,66 +1108,66 @@
       <c r="G14" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
+      <c r="H14" t="str">
+        <v>1ZA6071R0491392305</v>
+      </c>
+      <c r="I14" t="str">
+        <v>53.26</v>
+      </c>
       <c r="J14" t="str">
         <v>UPS</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>44769</v>
+        <v>44758</v>
       </c>
       <c r="B15" t="str">
-        <v>44777</v>
+        <v>44784</v>
       </c>
       <c r="C15" t="str">
-        <v>360</v>
+        <v>160</v>
       </c>
       <c r="D15" t="str">
-        <v>Fire</v>
+        <v>Ether</v>
       </c>
       <c r="E15" t="str">
-        <v>Mary Casey Bowers</v>
+        <v>Kristina Danelian</v>
       </c>
       <c r="F15" t="str">
-        <v>United States</v>
+        <v>Italia</v>
       </c>
       <c r="G15" t="str">
-        <v xml:space="preserve"> Etsy</v>
+        <v>Insta</v>
       </c>
       <c r="H15" t="str">
-        <v>1ZA6071R0491392305</v>
-      </c>
-      <c r="I15" t="str">
-        <v>53.26</v>
+        <v>RH068819076UA</v>
       </c>
       <c r="J15" t="str">
-        <v>UPS</v>
+        <v>UkrPoshta</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>44758</v>
+        <v>44753</v>
       </c>
       <c r="B16" t="str">
-        <v>44784</v>
+        <v>44767</v>
       </c>
       <c r="C16" t="str">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="D16" t="str">
-        <v>Ether</v>
+        <v>Fire</v>
       </c>
       <c r="E16" t="str">
-        <v>Kristina Danelian</v>
+        <v>Maggie Friedman</v>
       </c>
       <c r="F16" t="str">
-        <v>Italia</v>
+        <v>United Kingdom</v>
       </c>
       <c r="G16" t="str">
-        <v>Insta</v>
-      </c>
-      <c r="H16" t="str">
-        <v>RH068819076UA</v>
+        <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="J16" t="str">
         <v>UkrPoshta</v>
@@ -1123,48 +1175,48 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>44753</v>
-      </c>
-      <c r="B17" t="str">
-        <v>44767</v>
+        <v>44743</v>
       </c>
       <c r="C17" t="str">
-        <v>360</v>
-      </c>
-      <c r="D17" t="str">
-        <v>Fire</v>
+        <v>240</v>
       </c>
       <c r="E17" t="str">
-        <v>Maggie Friedman</v>
+        <v>Вікторія Поларуш</v>
       </c>
       <c r="F17" t="str">
-        <v>United Kingdom</v>
+        <v>Польща</v>
       </c>
       <c r="G17" t="str">
-        <v xml:space="preserve"> Etsy</v>
+        <v>Facebook</v>
       </c>
       <c r="J17" t="str">
-        <v>UkrPoshta</v>
+        <v>Курьер</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
         <v>44743</v>
       </c>
+      <c r="B18" t="str">
+        <v>44777</v>
+      </c>
       <c r="C18" t="str">
-        <v>240</v>
+        <v>87</v>
+      </c>
+      <c r="D18" t="str">
+        <v>3 Чохла</v>
       </c>
       <c r="E18" t="str">
-        <v>Вікторія Поларуш</v>
+        <v>Alla Michailidou</v>
       </c>
       <c r="F18" t="str">
-        <v>Польща</v>
-      </c>
-      <c r="G18" t="str">
-        <v>Facebook</v>
+        <v>Cyprus</v>
+      </c>
+      <c r="H18" t="str">
+        <v>CP067745099UA</v>
       </c>
       <c r="J18" t="str">
-        <v>Курьер</v>
+        <v>UkrPoshta</v>
       </c>
     </row>
     <row r="19">
@@ -1175,10 +1227,10 @@
         <v>44777</v>
       </c>
       <c r="C19" t="str">
-        <v>87</v>
+        <v>216</v>
       </c>
       <c r="D19" t="str">
-        <v>3 Чохла</v>
+        <v>Ether</v>
       </c>
       <c r="E19" t="str">
         <v>Alla Michailidou</v>
@@ -1188,9 +1240,6 @@
       </c>
       <c r="H19" t="str">
         <v>CP067745099UA</v>
-      </c>
-      <c r="J19" t="str">
-        <v>UkrPoshta</v>
       </c>
     </row>
     <row r="20">
@@ -1204,7 +1253,7 @@
         <v>216</v>
       </c>
       <c r="D20" t="str">
-        <v>Ether</v>
+        <v>Alchemy</v>
       </c>
       <c r="E20" t="str">
         <v>Alla Michailidou</v>
@@ -1212,66 +1261,62 @@
       <c r="F20" t="str">
         <v>Cyprus</v>
       </c>
-      <c r="H20" t="str">
-        <v>CP067745099UA</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>44743</v>
-      </c>
-      <c r="B21" t="str">
-        <v>44777</v>
-      </c>
-      <c r="C21" t="str">
-        <v>216</v>
-      </c>
-      <c r="D21" t="str">
-        <v>Alchemy</v>
-      </c>
-      <c r="E21" t="str">
-        <v>Alla Michailidou</v>
-      </c>
-      <c r="F21" t="str">
-        <v>Cyprus</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A2:J21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J20"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G21"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
-    <row r="2">
-      <c r="A2" t="str">
+    <row r="1">
+      <c r="A1" t="str">
         <v>Дата оплаты</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B1" t="str">
         <v>Сумма</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C1" t="str">
         <v>Описание</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D1" t="str">
         <v>Номер телефона, соцсети</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E1" t="str">
         <v>Имя покупателя</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F1" t="str">
         <v>Адрес покупателя</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G1" t="str">
         <v>Откуда покупатель</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>44789</v>
+      </c>
+      <c r="B3" t="str">
+        <v>5000</v>
+      </c>
+      <c r="C3" t="str">
+        <v xml:space="preserve">Infinity </v>
+      </c>
+      <c r="E3" t="str">
+        <v>Yogaist</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Київ</v>
+      </c>
+      <c r="G3" t="str">
+        <v xml:space="preserve">Instagram </v>
       </c>
     </row>
     <row r="4">
@@ -1279,19 +1324,16 @@
         <v>44789</v>
       </c>
       <c r="B4" t="str">
-        <v>5000</v>
+        <v>5500</v>
       </c>
       <c r="C4" t="str">
-        <v xml:space="preserve">Infinity </v>
+        <v xml:space="preserve">Eternal love </v>
       </c>
       <c r="E4" t="str">
-        <v>Yogaist</v>
+        <v xml:space="preserve">Аліна Єгорова </v>
       </c>
       <c r="F4" t="str">
-        <v>Київ</v>
-      </c>
-      <c r="G4" t="str">
-        <v xml:space="preserve">Instagram </v>
+        <v>Дніпро</v>
       </c>
     </row>
     <row r="5">
@@ -1299,113 +1341,116 @@
         <v>44789</v>
       </c>
       <c r="B5" t="str">
-        <v>5500</v>
+        <v>5250</v>
       </c>
       <c r="C5" t="str">
-        <v xml:space="preserve">Eternal love </v>
+        <v>Fire</v>
       </c>
       <c r="E5" t="str">
-        <v xml:space="preserve">Аліна Єгорова </v>
+        <v>Марина</v>
       </c>
       <c r="F5" t="str">
-        <v>Дніпро</v>
+        <v>Львів</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Артур Никоненко</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>44789</v>
+        <v>44788</v>
       </c>
       <c r="B6" t="str">
-        <v>5250</v>
+        <v>5500</v>
       </c>
       <c r="C6" t="str">
-        <v>Fire</v>
+        <v xml:space="preserve">Ether wood </v>
       </c>
       <c r="E6" t="str">
-        <v>Марина</v>
+        <v>Антон Тсовма</v>
       </c>
       <c r="F6" t="str">
         <v>Львів</v>
       </c>
       <c r="G6" t="str">
-        <v>Артур Никоненко</v>
+        <v>Тизенберг Р.</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>44788</v>
+        <v>44785</v>
       </c>
       <c r="B7" t="str">
         <v>5500</v>
       </c>
       <c r="C7" t="str">
-        <v xml:space="preserve">Ether wood </v>
+        <v xml:space="preserve">Eternal love </v>
       </c>
       <c r="E7" t="str">
-        <v>Антон Тсовма</v>
+        <v>Ліна</v>
       </c>
       <c r="F7" t="str">
-        <v>Львів</v>
+        <v>Київ</v>
       </c>
       <c r="G7" t="str">
-        <v>Тизенберг Р.</v>
+        <v xml:space="preserve">Instagram </v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>44785</v>
+        <v>44775</v>
       </c>
       <c r="B8" t="str">
-        <v>5500</v>
+        <v>4500</v>
       </c>
       <c r="C8" t="str">
-        <v xml:space="preserve">Eternal love </v>
+        <v>Infinity</v>
       </c>
       <c r="E8" t="str">
-        <v>Ліна</v>
+        <v>Олена Кареліна</v>
       </c>
       <c r="F8" t="str">
         <v>Київ</v>
       </c>
-      <c r="G8" t="str">
-        <v xml:space="preserve">Instagram </v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>44775</v>
+        <v>44780</v>
       </c>
       <c r="B9" t="str">
-        <v>4500</v>
+        <v>5500</v>
       </c>
       <c r="C9" t="str">
-        <v>Infinity</v>
+        <v xml:space="preserve">Eternal love </v>
       </c>
       <c r="E9" t="str">
-        <v>Олена Кареліна</v>
+        <v>Yogaist</v>
       </c>
       <c r="F9" t="str">
         <v>Київ</v>
       </c>
+      <c r="G9" t="str">
+        <v xml:space="preserve">Instagram </v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>44780</v>
+        <v>44771</v>
       </c>
       <c r="B10" t="str">
         <v>5500</v>
       </c>
       <c r="C10" t="str">
-        <v xml:space="preserve">Eternal love </v>
+        <v>Fire</v>
       </c>
       <c r="E10" t="str">
-        <v>Yogaist</v>
+        <v>Ольга</v>
       </c>
       <c r="F10" t="str">
         <v>Київ</v>
       </c>
       <c r="G10" t="str">
-        <v xml:space="preserve">Instagram </v>
+        <v>Instagram</v>
       </c>
     </row>
     <row r="11">
@@ -1413,19 +1458,16 @@
         <v>44771</v>
       </c>
       <c r="B11" t="str">
-        <v>5500</v>
+        <v>4500</v>
       </c>
       <c r="C11" t="str">
         <v>Fire</v>
       </c>
       <c r="E11" t="str">
-        <v>Ольга</v>
+        <v>Алексанр Пилипчук</v>
       </c>
       <c r="F11" t="str">
-        <v>Київ</v>
-      </c>
-      <c r="G11" t="str">
-        <v>Instagram</v>
+        <v>Львів</v>
       </c>
     </row>
     <row r="12">
@@ -1436,7 +1478,7 @@
         <v>4500</v>
       </c>
       <c r="C12" t="str">
-        <v>Fire</v>
+        <v>Alchemy</v>
       </c>
       <c r="E12" t="str">
         <v>Алексанр Пилипчук</v>
@@ -1470,7 +1512,7 @@
         <v>4500</v>
       </c>
       <c r="C14" t="str">
-        <v>Alchemy</v>
+        <v>Ether</v>
       </c>
       <c r="E14" t="str">
         <v>Алексанр Пилипчук</v>
@@ -1481,19 +1523,16 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>44771</v>
+        <v>44766</v>
       </c>
       <c r="B15" t="str">
-        <v>4500</v>
+        <v>4675</v>
       </c>
       <c r="C15" t="str">
-        <v>Ether</v>
-      </c>
-      <c r="E15" t="str">
-        <v>Алексанр Пилипчук</v>
-      </c>
-      <c r="F15" t="str">
-        <v>Львів</v>
+        <v>Fire</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Хоттей</v>
       </c>
     </row>
     <row r="16">
@@ -1507,7 +1546,7 @@
         <v>Fire</v>
       </c>
       <c r="G16" t="str">
-        <v>Хоттей</v>
+        <v>Сазанова Н.</v>
       </c>
     </row>
     <row r="17">
@@ -1515,13 +1554,13 @@
         <v>44766</v>
       </c>
       <c r="B17" t="str">
-        <v>4675</v>
+        <v>3000</v>
       </c>
       <c r="C17" t="str">
-        <v>Fire</v>
-      </c>
-      <c r="G17" t="str">
-        <v>Сазанова Н.</v>
+        <v>Ether</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Александр Ананда</v>
       </c>
     </row>
     <row r="18">
@@ -1529,27 +1568,24 @@
         <v>44766</v>
       </c>
       <c r="B18" t="str">
-        <v>3000</v>
+        <v>4200</v>
       </c>
       <c r="C18" t="str">
         <v>Ether</v>
       </c>
       <c r="E18" t="str">
-        <v>Александр Ананда</v>
+        <v>Добриня</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>44766</v>
+        <v>44756</v>
       </c>
       <c r="B19" t="str">
-        <v>4200</v>
-      </c>
-      <c r="C19" t="str">
-        <v>Ether</v>
-      </c>
-      <c r="E19" t="str">
-        <v>Добриня</v>
+        <v>4775</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Стульнікова</v>
       </c>
     </row>
     <row r="20">
@@ -1563,21 +1599,9 @@
         <v>Стульнікова</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>44756</v>
-      </c>
-      <c r="B21" t="str">
-        <v>4775</v>
-      </c>
-      <c r="G21" t="str">
-        <v>Стульнікова</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A2:G21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add class Table; class Sheet; some fix
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -406,13 +406,6 @@
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -722,9 +715,6 @@
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -795,7 +785,7 @@
         <v>Подставки</v>
       </c>
       <c r="B9">
-        <v>-2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -859,7 +849,7 @@
         <v>Паракорд бордо 48 см</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
@@ -1019,7 +1009,7 @@
         <v>Стикеры</v>
       </c>
       <c r="B37">
-        <v>106</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">

</xml_diff>

<commit_message>
set and get last change date
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="ready_to_sale" sheetId="1" r:id="rId1"/>
     <sheet name="tubes" sheetId="2" r:id="rId2"/>
@@ -402,17 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -430,38 +423,44 @@
       <c r="E1" t="str">
         <v>Бронь UA</v>
       </c>
+      <c r="F1" t="str">
+        <v>Date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Fire</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="str">
         <v>15</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="C2" t="str">
+        <v>30</v>
+      </c>
+      <c r="D2" t="str">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Waterfall</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="C3" t="str">
+        <v>10</v>
+      </c>
+      <c r="D3" t="str">
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
         <v>0</v>
       </c>
     </row>
@@ -469,16 +468,16 @@
       <c r="A4" t="str">
         <v>Ether-Acril</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="C4" t="str">
+        <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
         <v>0</v>
       </c>
     </row>
@@ -486,16 +485,16 @@
       <c r="A5" t="str">
         <v>Ether-Wood</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="C5" t="str">
+        <v>0</v>
+      </c>
+      <c r="D5" t="str">
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
         <v>0</v>
       </c>
     </row>
@@ -503,16 +502,16 @@
       <c r="A6" t="str">
         <v>Alchemy</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="str">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D6" t="str">
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
         <v>0</v>
       </c>
     </row>
@@ -520,16 +519,16 @@
       <c r="A7" t="str">
         <v>Infinity</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
+      <c r="B7" t="str">
+        <v>0</v>
+      </c>
+      <c r="C7" t="str">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D7" t="str">
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
         <v>0</v>
       </c>
     </row>
@@ -537,32 +536,31 @@
       <c r="A8" t="str">
         <v>Eternal-love</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="str">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="D8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -572,20 +570,26 @@
       <c r="B1" t="str">
         <v>Количество</v>
       </c>
+      <c r="C1" t="str">
+        <v>Date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Fire</v>
       </c>
-      <c r="B2">
-        <v>5</v>
+      <c r="B2" t="str">
+        <v>15</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Waterfall</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
         <v>0</v>
       </c>
     </row>
@@ -593,7 +597,7 @@
       <c r="A4" t="str">
         <v>Ether-Acril</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
         <v>0</v>
       </c>
     </row>
@@ -601,7 +605,7 @@
       <c r="A5" t="str">
         <v>Ether-Wood</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
         <v>0</v>
       </c>
     </row>
@@ -609,7 +613,7 @@
       <c r="A6" t="str">
         <v>Alchemy</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="str">
         <v>0</v>
       </c>
     </row>
@@ -617,7 +621,7 @@
       <c r="A7" t="str">
         <v>Infinity</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
         <v>0</v>
       </c>
     </row>
@@ -625,23 +629,22 @@
       <c r="A8" t="str">
         <v>Eternal-love</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -651,20 +654,26 @@
       <c r="B1" t="str">
         <v>Количество</v>
       </c>
+      <c r="C1" t="str">
+        <v>Date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Fire</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="str">
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Waterfall</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
         <v>0</v>
       </c>
     </row>
@@ -672,7 +681,7 @@
       <c r="A4" t="str">
         <v>Ether-Acril</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
         <v>0</v>
       </c>
     </row>
@@ -680,7 +689,7 @@
       <c r="A5" t="str">
         <v>Ether-Wood</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="str">
         <v>0</v>
       </c>
     </row>
@@ -688,15 +697,15 @@
       <c r="A6" t="str">
         <v>Alchemy</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" t="str">
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>Infinity</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="str">
         <v>0</v>
       </c>
     </row>
@@ -704,27 +713,23 @@
       <c r="A8" t="str">
         <v>Eternal-love</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -733,20 +738,26 @@
       <c r="B1" t="str">
         <v>Количество</v>
       </c>
+      <c r="C1" t="str">
+        <v>Date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Bag стандарт</v>
       </c>
-      <c r="B2">
-        <v>37</v>
+      <c r="B2" t="str">
+        <v>-13</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Bag эфир</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="str">
         <v>43</v>
       </c>
     </row>
@@ -754,7 +765,7 @@
       <c r="A4" t="str">
         <v>Box Divya</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="str">
         <v>119</v>
       </c>
     </row>
@@ -762,31 +773,31 @@
       <c r="A5" t="str">
         <v>Планки дерево Б</v>
       </c>
-      <c r="B5">
-        <v>15</v>
+      <c r="B5" t="str">
+        <v>-35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Планки дерево М</v>
       </c>
-      <c r="B6">
-        <v>3</v>
+      <c r="B6" t="str">
+        <v>-47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>Планки акрил Б</v>
       </c>
-      <c r="B7">
-        <v>9</v>
+      <c r="B7" t="str">
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>Планки акрил М</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <v>8</v>
       </c>
     </row>
@@ -794,15 +805,15 @@
       <c r="A9" t="str">
         <v>Подставки</v>
       </c>
-      <c r="B9">
-        <v>-2</v>
+      <c r="B9" t="str">
+        <v>-52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
         <v>Подставки акрил</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="str">
         <v>2</v>
       </c>
     </row>
@@ -810,23 +821,23 @@
       <c r="A11" t="str">
         <v>Стики</v>
       </c>
-      <c r="B11">
-        <v>2</v>
+      <c r="B11" t="str">
+        <v>-48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
         <v>Флизелин стандарт</v>
       </c>
-      <c r="B12">
-        <v>27</v>
+      <c r="B12" t="str">
+        <v>-23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
         <v>Флизелин Ефир</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="str">
         <v>20</v>
       </c>
     </row>
@@ -834,7 +845,7 @@
       <c r="A14" t="str">
         <v>Паракорд серый 35 см</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="str">
         <v>13</v>
       </c>
     </row>
@@ -842,7 +853,7 @@
       <c r="A15" t="str">
         <v>Паракорд серый 48 см</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="str">
         <v>12</v>
       </c>
     </row>
@@ -850,47 +861,47 @@
       <c r="A16" t="str">
         <v>Паракорд бордо 35 см</v>
       </c>
-      <c r="B16">
-        <v>7</v>
+      <c r="B16" t="str">
+        <v>-43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
         <v>Паракорд бордо 48 см</v>
       </c>
-      <c r="B17">
-        <v>9</v>
+      <c r="B17" t="str">
+        <v>-41</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
         <v>Миникорд серый 110 см</v>
       </c>
-      <c r="B18">
-        <v>29</v>
+      <c r="B18" t="str">
+        <v>-71</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
         <v>Шнур с карабином</v>
       </c>
-      <c r="B19">
-        <v>6</v>
+      <c r="B19" t="str">
+        <v>-44</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
         <v>Войлок 85х50 см</v>
       </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" t="str">
+        <v>25</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
         <v>Замша 80х50 см</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="str">
         <v>0</v>
       </c>
     </row>
@@ -898,7 +909,7 @@
       <c r="A22" t="str">
         <v>Карабины</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="str">
         <v>0</v>
       </c>
     </row>
@@ -906,7 +917,7 @@
       <c r="A23" t="str">
         <v>Чехлы для чаш</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="str">
         <v>0</v>
       </c>
     </row>
@@ -914,7 +925,7 @@
       <c r="A24" t="str">
         <v>Box чехлы для чаш</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="str">
         <v>21</v>
       </c>
     </row>
@@ -922,7 +933,7 @@
       <c r="A25" t="str">
         <v>Паспорт Fire En</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="str">
         <v>29</v>
       </c>
     </row>
@@ -930,7 +941,7 @@
       <c r="A26" t="str">
         <v>Паспорт Ether En</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="str">
         <v>32</v>
       </c>
     </row>
@@ -938,7 +949,7 @@
       <c r="A27" t="str">
         <v>Паспорт Waterfall En</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="str">
         <v>27</v>
       </c>
     </row>
@@ -946,7 +957,7 @@
       <c r="A28" t="str">
         <v>Паспорт Alchemy En</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="str">
         <v>28</v>
       </c>
     </row>
@@ -954,7 +965,7 @@
       <c r="A29" t="str">
         <v>Паспорт Infinity En</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="str">
         <v>32</v>
       </c>
     </row>
@@ -962,7 +973,7 @@
       <c r="A30" t="str">
         <v>Паспорт Eternal Love En</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="str">
         <v>30</v>
       </c>
     </row>
@@ -970,7 +981,7 @@
       <c r="A31" t="str">
         <v>Паспорт Fire Ua</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="str">
         <v>35</v>
       </c>
     </row>
@@ -978,7 +989,7 @@
       <c r="A32" t="str">
         <v>Паспорт Ether Ua</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="str">
         <v>40</v>
       </c>
     </row>
@@ -986,7 +997,7 @@
       <c r="A33" t="str">
         <v>Паспорт Waterfall Ua</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="str">
         <v>39</v>
       </c>
     </row>
@@ -994,7 +1005,7 @@
       <c r="A34" t="str">
         <v>Паспорт Alchemy Ua</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="str">
         <v>32</v>
       </c>
     </row>
@@ -1002,7 +1013,7 @@
       <c r="A35" t="str">
         <v>Паспорт Infinity Ua</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="str">
         <v>29</v>
       </c>
     </row>
@@ -1010,7 +1021,7 @@
       <c r="A36" t="str">
         <v>Пacпорт Eternal Love Ua</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="str">
         <v>33</v>
       </c>
     </row>
@@ -1018,7 +1029,7 @@
       <c r="A37" t="str">
         <v>Стикеры</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="str">
         <v>106</v>
       </c>
     </row>
@@ -1026,74 +1037,99 @@
       <c r="A38" t="str">
         <v>Наклейки на коробки</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="str">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B38"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C38"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
+    <row r="1" xml:space="preserve">
+      <c r="A1" t="str">
         <v>Отправка</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B1" t="str">
         <v>Получение</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C1" t="str">
         <v xml:space="preserve">Сумма </v>
       </c>
-      <c r="D2" t="str">
+      <c r="D1" t="str">
         <v>Описание</v>
       </c>
-      <c r="E2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Имя_x000d__x000d__x000d__x000d__x000d_
+      <c r="E1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Имя_x000d_
 покупателя</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F1" t="str">
         <v>Страна</v>
       </c>
-      <c r="G2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Откуда_x000d__x000d__x000d__x000d__x000d_
+      <c r="G1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Откуда_x000d_
 покупатель</v>
       </c>
-      <c r="H2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Track_x000d__x000d__x000d__x000d__x000d_
+      <c r="H1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Track_x000d_
 number</v>
       </c>
-      <c r="I2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Стоимость_x000d__x000d__x000d__x000d__x000d_
+      <c r="I1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Стоимость_x000d_
 доставки</v>
       </c>
-      <c r="J2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Почтовая_x000d__x000d__x000d__x000d__x000d_
+      <c r="J1" t="str" xml:space="preserve">
+        <v xml:space="preserve">Почтовая_x000d_
 служба</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>44790</v>
+      </c>
+      <c r="C5" t="str">
+        <v>360</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Infinity</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Vasile Christian</v>
+      </c>
+      <c r="F5" t="str">
+        <v>United States</v>
+      </c>
+      <c r="G5" t="str">
+        <v xml:space="preserve"> Etsy</v>
+      </c>
+      <c r="H5" t="str">
+        <v>1ZA6071R0497715606</v>
+      </c>
+      <c r="J5" t="str">
+        <v>UPS</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>44790</v>
+        <v>44789</v>
       </c>
       <c r="C6" t="str">
         <v>360</v>
       </c>
       <c r="D6" t="str">
-        <v>Infinity</v>
+        <v>Alchemy</v>
       </c>
       <c r="E6" t="str">
-        <v>Vasile Christian</v>
+        <v>WILLIAM M GUAY</v>
       </c>
       <c r="F6" t="str">
         <v>United States</v>
@@ -1102,7 +1138,7 @@
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H6" t="str">
-        <v>1ZA6071R0497715606</v>
+        <v>1ZA6071R0494460726</v>
       </c>
       <c r="J6" t="str">
         <v>UPS</v>
@@ -1116,19 +1152,19 @@
         <v>360</v>
       </c>
       <c r="D7" t="str">
-        <v>Alchemy</v>
+        <v>Waterfall</v>
       </c>
       <c r="E7" t="str">
-        <v>WILLIAM M GUAY</v>
+        <v>Yulia Malkin</v>
       </c>
       <c r="F7" t="str">
-        <v>United States</v>
+        <v>Canada</v>
       </c>
       <c r="G7" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H7" t="str">
-        <v>1ZA6071R0494460726</v>
+        <v>1ZA6071R0491898117</v>
       </c>
       <c r="J7" t="str">
         <v>UPS</v>
@@ -1136,25 +1172,25 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>44789</v>
+        <v>44782</v>
       </c>
       <c r="C8" t="str">
         <v>360</v>
       </c>
       <c r="D8" t="str">
-        <v>Waterfall</v>
+        <v>Ether</v>
       </c>
       <c r="E8" t="str">
-        <v>Yulia Malkin</v>
+        <v>Tom Brouwer</v>
       </c>
       <c r="F8" t="str">
-        <v>Canada</v>
+        <v>Netherlands</v>
       </c>
       <c r="G8" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H8" t="str">
-        <v>1ZA6071R0491898117</v>
+        <v>1ZA6071R0491977602</v>
       </c>
       <c r="J8" t="str">
         <v>UPS</v>
@@ -1162,28 +1198,25 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>44782</v>
+        <v>44776</v>
+      </c>
+      <c r="B9" t="str">
+        <v>44784</v>
       </c>
       <c r="C9" t="str">
         <v>360</v>
       </c>
       <c r="D9" t="str">
-        <v>Ether</v>
+        <v>Fire</v>
       </c>
       <c r="E9" t="str">
-        <v>Tom Brouwer</v>
+        <v>Paul Chek</v>
       </c>
       <c r="F9" t="str">
-        <v>Netherlands</v>
+        <v>United States</v>
       </c>
       <c r="G9" t="str">
         <v xml:space="preserve"> Etsy</v>
-      </c>
-      <c r="H9" t="str">
-        <v>1ZA6071R0491977602</v>
-      </c>
-      <c r="J9" t="str">
-        <v>UPS</v>
       </c>
     </row>
     <row r="10">
@@ -1197,77 +1230,86 @@
         <v>360</v>
       </c>
       <c r="D10" t="str">
-        <v>Fire</v>
+        <v>Infinity</v>
       </c>
       <c r="E10" t="str">
-        <v>Paul Chek</v>
+        <v>Stephen Huggins</v>
       </c>
       <c r="F10" t="str">
         <v>United States</v>
       </c>
       <c r="G10" t="str">
         <v xml:space="preserve"> Etsy</v>
+      </c>
+      <c r="H10" t="str">
+        <v>1ZA6071R0493815756</v>
+      </c>
+      <c r="I10" t="str">
+        <v>$ 53.68</v>
+      </c>
+      <c r="J10" t="str">
+        <v>UPS</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
         <v>44776</v>
       </c>
-      <c r="B11" t="str">
-        <v>44784</v>
-      </c>
       <c r="C11" t="str">
         <v>360</v>
       </c>
       <c r="D11" t="str">
-        <v>Infinity</v>
+        <v>Fire</v>
       </c>
       <c r="E11" t="str">
-        <v>Stephen Huggins</v>
+        <v>Veselina Popova</v>
       </c>
       <c r="F11" t="str">
-        <v>United States</v>
+        <v>France</v>
       </c>
       <c r="G11" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H11" t="str">
-        <v>1ZA6071R0493815756</v>
+        <v>RH069864023UA</v>
       </c>
       <c r="I11" t="str">
-        <v>$ 53.68</v>
+        <v>$ 24.75</v>
       </c>
       <c r="J11" t="str">
-        <v>UPS</v>
+        <v>UkrPoshta</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>44776</v>
+        <v>44769</v>
+      </c>
+      <c r="B12" t="str">
+        <v>44777</v>
       </c>
       <c r="C12" t="str">
         <v>360</v>
       </c>
       <c r="D12" t="str">
-        <v>Fire</v>
+        <v>Ether</v>
       </c>
       <c r="E12" t="str">
-        <v>Veselina Popova</v>
+        <v>Fawntice McCain</v>
       </c>
       <c r="F12" t="str">
-        <v>France</v>
+        <v>United States</v>
       </c>
       <c r="G12" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="H12" t="str">
-        <v>RH069864023UA</v>
+        <v>1ZA6071R0493130987</v>
       </c>
       <c r="I12" t="str">
-        <v>$ 24.75</v>
+        <v>76.54</v>
       </c>
       <c r="J12" t="str">
-        <v>UkrPoshta</v>
+        <v>UPS</v>
       </c>
     </row>
     <row r="13">
@@ -1281,7 +1323,7 @@
         <v>360</v>
       </c>
       <c r="D13" t="str">
-        <v>Ether</v>
+        <v>Waterfall</v>
       </c>
       <c r="E13" t="str">
         <v>Fawntice McCain</v>
@@ -1291,12 +1333,6 @@
       </c>
       <c r="G13" t="str">
         <v xml:space="preserve"> Etsy</v>
-      </c>
-      <c r="H13" t="str">
-        <v>1ZA6071R0493130987</v>
-      </c>
-      <c r="I13" t="str">
-        <v>76.54</v>
       </c>
       <c r="J13" t="str">
         <v>UPS</v>
@@ -1313,10 +1349,10 @@
         <v>360</v>
       </c>
       <c r="D14" t="str">
-        <v>Waterfall</v>
+        <v>Fire</v>
       </c>
       <c r="E14" t="str">
-        <v>Fawntice McCain</v>
+        <v>Mary Casey Bowers</v>
       </c>
       <c r="F14" t="str">
         <v>United States</v>
@@ -1324,66 +1360,66 @@
       <c r="G14" t="str">
         <v xml:space="preserve"> Etsy</v>
       </c>
+      <c r="H14" t="str">
+        <v>1ZA6071R0491392305</v>
+      </c>
+      <c r="I14" t="str">
+        <v>53.26</v>
+      </c>
       <c r="J14" t="str">
         <v>UPS</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>44769</v>
+        <v>44758</v>
       </c>
       <c r="B15" t="str">
-        <v>44777</v>
+        <v>44784</v>
       </c>
       <c r="C15" t="str">
-        <v>360</v>
+        <v>160</v>
       </c>
       <c r="D15" t="str">
-        <v>Fire</v>
+        <v>Ether</v>
       </c>
       <c r="E15" t="str">
-        <v>Mary Casey Bowers</v>
+        <v>Kristina Danelian</v>
       </c>
       <c r="F15" t="str">
-        <v>United States</v>
+        <v>Italia</v>
       </c>
       <c r="G15" t="str">
-        <v xml:space="preserve"> Etsy</v>
+        <v>Insta</v>
       </c>
       <c r="H15" t="str">
-        <v>1ZA6071R0491392305</v>
-      </c>
-      <c r="I15" t="str">
-        <v>53.26</v>
+        <v>RH068819076UA</v>
       </c>
       <c r="J15" t="str">
-        <v>UPS</v>
+        <v>UkrPoshta</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>44758</v>
+        <v>44753</v>
       </c>
       <c r="B16" t="str">
-        <v>44784</v>
+        <v>44767</v>
       </c>
       <c r="C16" t="str">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="D16" t="str">
-        <v>Ether</v>
+        <v>Fire</v>
       </c>
       <c r="E16" t="str">
-        <v>Kristina Danelian</v>
+        <v>Maggie Friedman</v>
       </c>
       <c r="F16" t="str">
-        <v>Italia</v>
+        <v>United Kingdom</v>
       </c>
       <c r="G16" t="str">
-        <v>Insta</v>
-      </c>
-      <c r="H16" t="str">
-        <v>RH068819076UA</v>
+        <v xml:space="preserve"> Etsy</v>
       </c>
       <c r="J16" t="str">
         <v>UkrPoshta</v>
@@ -1391,48 +1427,48 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>44753</v>
-      </c>
-      <c r="B17" t="str">
-        <v>44767</v>
+        <v>44743</v>
       </c>
       <c r="C17" t="str">
-        <v>360</v>
-      </c>
-      <c r="D17" t="str">
-        <v>Fire</v>
+        <v>240</v>
       </c>
       <c r="E17" t="str">
-        <v>Maggie Friedman</v>
+        <v>Вікторія Поларуш</v>
       </c>
       <c r="F17" t="str">
-        <v>United Kingdom</v>
+        <v>Польща</v>
       </c>
       <c r="G17" t="str">
-        <v xml:space="preserve"> Etsy</v>
+        <v>Facebook</v>
       </c>
       <c r="J17" t="str">
-        <v>UkrPoshta</v>
+        <v>Курьер</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
         <v>44743</v>
       </c>
+      <c r="B18" t="str">
+        <v>44777</v>
+      </c>
       <c r="C18" t="str">
-        <v>240</v>
+        <v>87</v>
+      </c>
+      <c r="D18" t="str">
+        <v>3 Чохла</v>
       </c>
       <c r="E18" t="str">
-        <v>Вікторія Поларуш</v>
+        <v>Alla Michailidou</v>
       </c>
       <c r="F18" t="str">
-        <v>Польща</v>
-      </c>
-      <c r="G18" t="str">
-        <v>Facebook</v>
+        <v>Cyprus</v>
+      </c>
+      <c r="H18" t="str">
+        <v>CP067745099UA</v>
       </c>
       <c r="J18" t="str">
-        <v>Курьер</v>
+        <v>UkrPoshta</v>
       </c>
     </row>
     <row r="19">
@@ -1443,10 +1479,10 @@
         <v>44777</v>
       </c>
       <c r="C19" t="str">
-        <v>87</v>
+        <v>216</v>
       </c>
       <c r="D19" t="str">
-        <v>3 Чохла</v>
+        <v>Ether</v>
       </c>
       <c r="E19" t="str">
         <v>Alla Michailidou</v>
@@ -1456,9 +1492,6 @@
       </c>
       <c r="H19" t="str">
         <v>CP067745099UA</v>
-      </c>
-      <c r="J19" t="str">
-        <v>UkrPoshta</v>
       </c>
     </row>
     <row r="20">
@@ -1472,7 +1505,7 @@
         <v>216</v>
       </c>
       <c r="D20" t="str">
-        <v>Ether</v>
+        <v>Alchemy</v>
       </c>
       <c r="E20" t="str">
         <v>Alla Michailidou</v>
@@ -1480,66 +1513,62 @@
       <c r="F20" t="str">
         <v>Cyprus</v>
       </c>
-      <c r="H20" t="str">
-        <v>CP067745099UA</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>44743</v>
-      </c>
-      <c r="B21" t="str">
-        <v>44777</v>
-      </c>
-      <c r="C21" t="str">
-        <v>216</v>
-      </c>
-      <c r="D21" t="str">
-        <v>Alchemy</v>
-      </c>
-      <c r="E21" t="str">
-        <v>Alla Michailidou</v>
-      </c>
-      <c r="F21" t="str">
-        <v>Cyprus</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A2:J21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J20"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G21"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
-    <row r="2">
-      <c r="A2" t="str">
+    <row r="1">
+      <c r="A1" t="str">
         <v>Дата оплаты</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B1" t="str">
         <v>Сумма</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C1" t="str">
         <v>Описание</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D1" t="str">
         <v>Номер телефона, соцсети</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E1" t="str">
         <v>Имя покупателя</v>
       </c>
-      <c r="F2" t="str">
+      <c r="F1" t="str">
         <v>Адрес покупателя</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G1" t="str">
         <v>Откуда покупатель</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>44789</v>
+      </c>
+      <c r="B3" t="str">
+        <v>5000</v>
+      </c>
+      <c r="C3" t="str">
+        <v xml:space="preserve">Infinity </v>
+      </c>
+      <c r="E3" t="str">
+        <v>Yogaist</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Київ</v>
+      </c>
+      <c r="G3" t="str">
+        <v xml:space="preserve">Instagram </v>
       </c>
     </row>
     <row r="4">
@@ -1547,19 +1576,16 @@
         <v>44789</v>
       </c>
       <c r="B4" t="str">
-        <v>5000</v>
+        <v>5500</v>
       </c>
       <c r="C4" t="str">
-        <v xml:space="preserve">Infinity </v>
+        <v xml:space="preserve">Eternal love </v>
       </c>
       <c r="E4" t="str">
-        <v>Yogaist</v>
+        <v xml:space="preserve">Аліна Єгорова </v>
       </c>
       <c r="F4" t="str">
-        <v>Київ</v>
-      </c>
-      <c r="G4" t="str">
-        <v xml:space="preserve">Instagram </v>
+        <v>Дніпро</v>
       </c>
     </row>
     <row r="5">
@@ -1567,113 +1593,116 @@
         <v>44789</v>
       </c>
       <c r="B5" t="str">
-        <v>5500</v>
+        <v>5250</v>
       </c>
       <c r="C5" t="str">
-        <v xml:space="preserve">Eternal love </v>
+        <v>Fire</v>
       </c>
       <c r="E5" t="str">
-        <v xml:space="preserve">Аліна Єгорова </v>
+        <v>Марина</v>
       </c>
       <c r="F5" t="str">
-        <v>Дніпро</v>
+        <v>Львів</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Артур Никоненко</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>44789</v>
+        <v>44788</v>
       </c>
       <c r="B6" t="str">
-        <v>5250</v>
+        <v>5500</v>
       </c>
       <c r="C6" t="str">
-        <v>Fire</v>
+        <v xml:space="preserve">Ether wood </v>
       </c>
       <c r="E6" t="str">
-        <v>Марина</v>
+        <v>Антон Тсовма</v>
       </c>
       <c r="F6" t="str">
         <v>Львів</v>
       </c>
       <c r="G6" t="str">
-        <v>Артур Никоненко</v>
+        <v>Тизенберг Р.</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>44788</v>
+        <v>44785</v>
       </c>
       <c r="B7" t="str">
         <v>5500</v>
       </c>
       <c r="C7" t="str">
-        <v xml:space="preserve">Ether wood </v>
+        <v xml:space="preserve">Eternal love </v>
       </c>
       <c r="E7" t="str">
-        <v>Антон Тсовма</v>
+        <v>Ліна</v>
       </c>
       <c r="F7" t="str">
-        <v>Львів</v>
+        <v>Київ</v>
       </c>
       <c r="G7" t="str">
-        <v>Тизенберг Р.</v>
+        <v xml:space="preserve">Instagram </v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>44785</v>
+        <v>44775</v>
       </c>
       <c r="B8" t="str">
-        <v>5500</v>
+        <v>4500</v>
       </c>
       <c r="C8" t="str">
-        <v xml:space="preserve">Eternal love </v>
+        <v>Infinity</v>
       </c>
       <c r="E8" t="str">
-        <v>Ліна</v>
+        <v>Олена Кареліна</v>
       </c>
       <c r="F8" t="str">
         <v>Київ</v>
       </c>
-      <c r="G8" t="str">
-        <v xml:space="preserve">Instagram </v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>44775</v>
+        <v>44780</v>
       </c>
       <c r="B9" t="str">
-        <v>4500</v>
+        <v>5500</v>
       </c>
       <c r="C9" t="str">
-        <v>Infinity</v>
+        <v xml:space="preserve">Eternal love </v>
       </c>
       <c r="E9" t="str">
-        <v>Олена Кареліна</v>
+        <v>Yogaist</v>
       </c>
       <c r="F9" t="str">
         <v>Київ</v>
       </c>
+      <c r="G9" t="str">
+        <v xml:space="preserve">Instagram </v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>44780</v>
+        <v>44771</v>
       </c>
       <c r="B10" t="str">
         <v>5500</v>
       </c>
       <c r="C10" t="str">
-        <v xml:space="preserve">Eternal love </v>
+        <v>Fire</v>
       </c>
       <c r="E10" t="str">
-        <v>Yogaist</v>
+        <v>Ольга</v>
       </c>
       <c r="F10" t="str">
         <v>Київ</v>
       </c>
       <c r="G10" t="str">
-        <v xml:space="preserve">Instagram </v>
+        <v>Instagram</v>
       </c>
     </row>
     <row r="11">
@@ -1681,19 +1710,16 @@
         <v>44771</v>
       </c>
       <c r="B11" t="str">
-        <v>5500</v>
+        <v>4500</v>
       </c>
       <c r="C11" t="str">
         <v>Fire</v>
       </c>
       <c r="E11" t="str">
-        <v>Ольга</v>
+        <v>Алексанр Пилипчук</v>
       </c>
       <c r="F11" t="str">
-        <v>Київ</v>
-      </c>
-      <c r="G11" t="str">
-        <v>Instagram</v>
+        <v>Львів</v>
       </c>
     </row>
     <row r="12">
@@ -1704,7 +1730,7 @@
         <v>4500</v>
       </c>
       <c r="C12" t="str">
-        <v>Fire</v>
+        <v>Alchemy</v>
       </c>
       <c r="E12" t="str">
         <v>Алексанр Пилипчук</v>
@@ -1738,7 +1764,7 @@
         <v>4500</v>
       </c>
       <c r="C14" t="str">
-        <v>Alchemy</v>
+        <v>Ether</v>
       </c>
       <c r="E14" t="str">
         <v>Алексанр Пилипчук</v>
@@ -1749,19 +1775,16 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>44771</v>
+        <v>44766</v>
       </c>
       <c r="B15" t="str">
-        <v>4500</v>
+        <v>4675</v>
       </c>
       <c r="C15" t="str">
-        <v>Ether</v>
-      </c>
-      <c r="E15" t="str">
-        <v>Алексанр Пилипчук</v>
-      </c>
-      <c r="F15" t="str">
-        <v>Львів</v>
+        <v>Fire</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Хоттей</v>
       </c>
     </row>
     <row r="16">
@@ -1775,7 +1798,7 @@
         <v>Fire</v>
       </c>
       <c r="G16" t="str">
-        <v>Хоттей</v>
+        <v>Сазанова Н.</v>
       </c>
     </row>
     <row r="17">
@@ -1783,13 +1806,13 @@
         <v>44766</v>
       </c>
       <c r="B17" t="str">
-        <v>4675</v>
+        <v>3000</v>
       </c>
       <c r="C17" t="str">
-        <v>Fire</v>
-      </c>
-      <c r="G17" t="str">
-        <v>Сазанова Н.</v>
+        <v>Ether</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Александр Ананда</v>
       </c>
     </row>
     <row r="18">
@@ -1797,27 +1820,24 @@
         <v>44766</v>
       </c>
       <c r="B18" t="str">
-        <v>3000</v>
+        <v>4200</v>
       </c>
       <c r="C18" t="str">
         <v>Ether</v>
       </c>
       <c r="E18" t="str">
-        <v>Александр Ананда</v>
+        <v>Добриня</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>44766</v>
+        <v>44756</v>
       </c>
       <c r="B19" t="str">
-        <v>4200</v>
-      </c>
-      <c r="C19" t="str">
-        <v>Ether</v>
-      </c>
-      <c r="E19" t="str">
-        <v>Добриня</v>
+        <v>4775</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Стульнікова</v>
       </c>
     </row>
     <row r="20">
@@ -1831,21 +1851,9 @@
         <v>Стульнікова</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>44756</v>
-      </c>
-      <c r="B21" t="str">
-        <v>4775</v>
-      </c>
-      <c r="G21" t="str">
-        <v>Стульнікова</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A2:G21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
writeOff_Passport fix; add writeOfTubes
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -438,7 +438,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="str">
         <v>0</v>
@@ -454,8 +454,8 @@
       <c r="A3" s="1" t="str">
         <v>Waterfall</v>
       </c>
-      <c r="B3" s="1" t="str">
-        <v>1</v>
+      <c r="B3" s="1">
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="str">
         <v>0</v>
@@ -474,8 +474,8 @@
       <c r="B4" s="1" t="str">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <v>0</v>
+      <c r="C4" s="1">
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="str">
         <v>0</v>
@@ -491,8 +491,8 @@
       <c r="B5" s="1" t="str">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="str">
-        <v>5</v>
+      <c r="C5" s="1">
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="str">
         <v>0</v>
@@ -540,9 +540,9 @@
         <v>Eternal-love</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="str">
         <v>11</v>
       </c>
       <c r="D8" s="1" t="str">
@@ -587,7 +587,7 @@
         <v>Waterfall</v>
       </c>
       <c r="B3" s="1" t="str">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -595,7 +595,7 @@
         <v>Ether-Acril</v>
       </c>
       <c r="B4" s="1" t="str">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -603,7 +603,7 @@
         <v>Ether-Wood</v>
       </c>
       <c r="B5" s="1" t="str">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -611,7 +611,7 @@
         <v>Alchemy</v>
       </c>
       <c r="B6" s="1" t="str">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -619,7 +619,7 @@
         <v>Infinity</v>
       </c>
       <c r="B7" s="1" t="str">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -627,7 +627,7 @@
         <v>Eternal-love</v>
       </c>
       <c r="B8" s="1" t="str">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -735,15 +735,15 @@
         <v>Bag стандарт</v>
       </c>
       <c r="B2" s="1">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
         <v>Bag эфир</v>
       </c>
-      <c r="B3" s="1" t="str">
-        <v>38</v>
+      <c r="B3" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -759,7 +759,7 @@
         <v>Планки дерево Б</v>
       </c>
       <c r="B5" s="1">
-        <v>-10</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="6">
@@ -767,23 +767,23 @@
         <v>Планки дерево М</v>
       </c>
       <c r="B6" s="1">
-        <v>-22</v>
+        <v>-37</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
         <v>Планки акрил Б</v>
       </c>
-      <c r="B7" s="1" t="str">
-        <v>9</v>
+      <c r="B7" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="str">
         <v>Планки акрил М</v>
       </c>
-      <c r="B8" s="1" t="str">
-        <v>8</v>
+      <c r="B8" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -791,15 +791,15 @@
         <v>Подставки</v>
       </c>
       <c r="B9" s="1">
-        <v>-17</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="str">
         <v>Подставки акрил</v>
       </c>
-      <c r="B10" s="1" t="str">
-        <v>2</v>
+      <c r="B10" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -807,7 +807,7 @@
         <v>Стики</v>
       </c>
       <c r="B11" s="1">
-        <v>-23</v>
+        <v>-39</v>
       </c>
     </row>
     <row r="12">
@@ -815,7 +815,7 @@
         <v>Флизелин стандарт</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="13">
@@ -830,16 +830,16 @@
       <c r="A14" s="1" t="str">
         <v>Паракорд серый 35 см</v>
       </c>
-      <c r="B14" s="1" t="str">
-        <v>13</v>
+      <c r="B14" s="1">
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="str">
         <v>Паракорд серый 48 см</v>
       </c>
-      <c r="B15" s="1" t="str">
-        <v>12</v>
+      <c r="B15" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="16">
@@ -847,7 +847,7 @@
         <v>Паракорд бордо 35 см</v>
       </c>
       <c r="B16" s="1">
-        <v>-18</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="17">
@@ -855,7 +855,7 @@
         <v>Паракорд бордо 48 см</v>
       </c>
       <c r="B17" s="1">
-        <v>9</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="18">
@@ -863,7 +863,7 @@
         <v>Миникорд серый 110 см</v>
       </c>
       <c r="B18" s="1">
-        <v>-21</v>
+        <v>-53</v>
       </c>
     </row>
     <row r="19">
@@ -871,7 +871,7 @@
         <v>Шнур с карабином</v>
       </c>
       <c r="B19" s="1">
-        <v>-19</v>
+        <v>-35</v>
       </c>
     </row>
     <row r="20">
@@ -919,7 +919,7 @@
         <v>Стикеры</v>
       </c>
       <c r="B25" s="1">
-        <v>-19</v>
+        <v>-35</v>
       </c>
     </row>
     <row r="26">
@@ -1769,11 +1769,11 @@
       <c r="A2" s="1" t="str">
         <v>Паспорт Fire</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="str">
         <v>28</v>
       </c>
       <c r="C2" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -1783,16 +1783,16 @@
       <c r="B3" s="1" t="str">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <v>35</v>
+      <c r="C3" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
         <v>Паспорт Waterfall</v>
       </c>
-      <c r="B4" s="1" t="str">
-        <v>27</v>
+      <c r="B4" s="1">
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="str">
         <v>39</v>
@@ -1824,10 +1824,10 @@
       <c r="A7" s="1" t="str">
         <v>Паспорт Eternal-Love</v>
       </c>
-      <c r="B7" s="1" t="str">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="1">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="str">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add last change date
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -435,10 +435,10 @@
         <v>Fire</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="C2" s="1">
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="str">
         <v>0</v>
@@ -447,18 +447,18 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="str">
-        <v>11.1.2023 2:25:40</v>
+        <v>21.01.2023 04:06</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
         <v>Waterfall</v>
       </c>
-      <c r="B3" s="1" t="str">
-        <v>3</v>
+      <c r="B3" s="1">
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="str">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="str">
         <v>0</v>
@@ -471,11 +471,11 @@
       <c r="A4" s="1" t="str">
         <v>Ether-Acril</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="str">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <v>1</v>
+      <c r="C4" s="1">
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="str">
         <v>0</v>
@@ -488,10 +488,10 @@
       <c r="A5" s="1" t="str">
         <v>Ether-Wood</v>
       </c>
-      <c r="B5" s="1" t="str">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="str">
         <v>15</v>
       </c>
       <c r="D5" s="1" t="str">
@@ -505,11 +505,11 @@
       <c r="A6" s="1" t="str">
         <v>Alchemy</v>
       </c>
-      <c r="B6" s="1">
-        <v>8</v>
+      <c r="B6" s="1" t="str">
+        <v>12</v>
       </c>
       <c r="C6" s="1">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="str">
         <v>0</v>
@@ -522,11 +522,11 @@
       <c r="A7" s="1" t="str">
         <v>Infinity</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="str">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <v>1</v>
+      <c r="C7" s="1">
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="str">
         <v>0</v>
@@ -542,7 +542,7 @@
       <c r="B8" s="1" t="str">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="str">
         <v>23</v>
       </c>
       <c r="D8" s="1" t="str">
@@ -561,7 +561,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -573,21 +573,27 @@
       <c r="B1" s="1" t="str">
         <v>Количество</v>
       </c>
+      <c r="C1" s="1" t="str">
+        <v>Date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
         <v>Fire</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>-4</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <v>21.01.2023 04:06</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="str">
         <v>Waterfall</v>
       </c>
-      <c r="B3" s="1" t="str">
-        <v>0</v>
+      <c r="B3" s="1">
+        <v>-8</v>
       </c>
     </row>
     <row r="4">
@@ -595,7 +601,7 @@
         <v>Ether</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="5">
@@ -603,7 +609,7 @@
         <v>Alchemy</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="6">
@@ -611,27 +617,27 @@
         <v>Infinity</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="str">
         <v>Eternal-love</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="str">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -643,6 +649,9 @@
       <c r="B1" s="1" t="str">
         <v>Количество</v>
       </c>
+      <c r="C1" s="1" t="str">
+        <v>Date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
@@ -702,14 +711,14 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -721,13 +730,19 @@
       <c r="B1" s="1" t="str">
         <v>Количество</v>
       </c>
+      <c r="C1" s="1" t="str">
+        <v>Date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
         <v>Bag стандарт</v>
       </c>
       <c r="B2" s="1">
-        <v>-39</v>
+        <v>-69</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <v>21.01.2023 04:06</v>
       </c>
     </row>
     <row r="3">
@@ -735,7 +750,7 @@
         <v>Bag эфир</v>
       </c>
       <c r="B3" s="1">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -751,7 +766,7 @@
         <v>Планки дерево Б</v>
       </c>
       <c r="B5" s="1">
-        <v>-76</v>
+        <v>-110</v>
       </c>
     </row>
     <row r="6">
@@ -759,7 +774,7 @@
         <v>Планки дерево М</v>
       </c>
       <c r="B6" s="1">
-        <v>-88</v>
+        <v>-122</v>
       </c>
     </row>
     <row r="7">
@@ -767,7 +782,7 @@
         <v>Планки акрил Б</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8">
@@ -775,7 +790,7 @@
         <v>Планки акрил М</v>
       </c>
       <c r="B8" s="1">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9">
@@ -783,7 +798,7 @@
         <v>Подставки</v>
       </c>
       <c r="B9" s="1">
-        <v>-83</v>
+        <v>-117</v>
       </c>
     </row>
     <row r="10">
@@ -791,7 +806,7 @@
         <v>Подставки акрил</v>
       </c>
       <c r="B10" s="1">
-        <v>-4</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="11">
@@ -799,7 +814,7 @@
         <v>Стики</v>
       </c>
       <c r="B11" s="1">
-        <v>-95</v>
+        <v>-133</v>
       </c>
     </row>
     <row r="12">
@@ -807,7 +822,10 @@
         <v>Флизелин стандарт</v>
       </c>
       <c r="B12" s="1">
-        <v>-70</v>
+        <v>-108</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -823,7 +841,7 @@
         <v>Паракорд серый 35 см</v>
       </c>
       <c r="B14" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -831,7 +849,7 @@
         <v>Паракорд серый 48 см</v>
       </c>
       <c r="B15" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -839,7 +857,7 @@
         <v>Паракорд бордо 35 см</v>
       </c>
       <c r="B16" s="1">
-        <v>-84</v>
+        <v>-118</v>
       </c>
     </row>
     <row r="17">
@@ -847,7 +865,7 @@
         <v>Паракорд бордо 48 см</v>
       </c>
       <c r="B17" s="1">
-        <v>-57</v>
+        <v>-91</v>
       </c>
     </row>
     <row r="18">
@@ -855,7 +873,7 @@
         <v>Миникорд серый 110 см</v>
       </c>
       <c r="B18" s="1">
-        <v>-165</v>
+        <v>-241</v>
       </c>
     </row>
     <row r="19">
@@ -863,7 +881,7 @@
         <v>Шнур с карабином</v>
       </c>
       <c r="B19" s="1">
-        <v>-91</v>
+        <v>-129</v>
       </c>
     </row>
     <row r="20">
@@ -911,7 +929,7 @@
         <v>Стикеры</v>
       </c>
       <c r="B25" s="1">
-        <v>-91</v>
+        <v>-129</v>
       </c>
     </row>
     <row r="26">
@@ -924,7 +942,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C26"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1741,7 +1759,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1756,16 +1774,22 @@
       <c r="C1" s="1" t="str">
         <v>В наличии UA</v>
       </c>
+      <c r="D1" s="1" t="str">
+        <v>Date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
         <v>Паспорт Fire</v>
       </c>
       <c r="B2" s="1" t="str">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="C2" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <v>21.01.2023 04:06</v>
       </c>
     </row>
     <row r="3">
@@ -1773,43 +1797,43 @@
         <v>Паспорт Ether</v>
       </c>
       <c r="B3" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="str">
         <v>Паспорт Waterfall</v>
       </c>
-      <c r="B4" s="1" t="str">
-        <v>25</v>
+      <c r="B4" s="1">
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="str">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="str">
         <v>Паспорт Alchemy</v>
       </c>
-      <c r="B5" s="1">
-        <v>21</v>
+      <c r="B5" s="1" t="str">
+        <v>17</v>
       </c>
       <c r="C5" s="1">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="str">
         <v>Паспорт Infinity</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="str">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <v>29</v>
+      <c r="C6" s="1">
+        <v>26</v>
       </c>
     </row>
     <row r="7">
@@ -1819,13 +1843,13 @@
       <c r="B7" s="1" t="str">
         <v>25</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="str">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write to table info about sales
</commit_message>
<xml_diff>
--- a/data/dataTable.xlsx
+++ b/data/dataTable.xlsx
@@ -10,6 +10,7 @@
     <sheet name="passports" sheetId="5" r:id="rId5"/>
     <sheet name="Sales" sheetId="6" r:id="rId6"/>
     <sheet name="Sales Ua" sheetId="7" r:id="rId7"/>
+    <sheet name="sales_bot" sheetId="8" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -407,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -438,7 +439,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="str">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D2" s="1" t="str">
         <v>0</v>
@@ -447,7 +448,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="str">
-        <v>31.07.2023 22:16</v>
+        <v>28.09.2023 01:55</v>
       </c>
     </row>
     <row r="3">
@@ -457,8 +458,8 @@
       <c r="B3" s="1" t="str">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <v>2</v>
+      <c r="C3" s="1">
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="str">
         <v>0</v>
@@ -492,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="str">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D5" s="1" t="str">
         <v>0</v>
@@ -522,11 +523,11 @@
       <c r="A7" s="1" t="str">
         <v>Infinity</v>
       </c>
-      <c r="B7" s="1" t="str">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="str">
-        <v>0</v>
+      <c r="B7" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-2</v>
       </c>
       <c r="D7" s="1" t="str">
         <v>0</v>
@@ -539,8 +540,8 @@
       <c r="A8" s="1" t="str">
         <v>Eternal-love</v>
       </c>
-      <c r="B8" s="1" t="str">
-        <v>2</v>
+      <c r="B8" s="1">
+        <v>-2</v>
       </c>
       <c r="C8" s="1" t="str">
         <v>0</v>
@@ -557,7 +558,7 @@
         <v>Golden-Gate</v>
       </c>
       <c r="B9" s="1" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="str">
         <v>0</v>
@@ -573,8 +574,8 @@
       <c r="A10" s="1" t="str">
         <v>Aerial</v>
       </c>
-      <c r="B10" s="1" t="str">
-        <v>1</v>
+      <c r="B10" s="1">
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="str">
         <v>1</v>
@@ -597,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -689,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -787,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1023,7 +1024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1142,7 +1143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1" xml:space="preserve">
@@ -1159,26 +1160,26 @@
         <v>Описание</v>
       </c>
       <c r="E1" s="1" t="str" xml:space="preserve">
-        <v xml:space="preserve">Имя_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Имя_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 покупателя</v>
       </c>
       <c r="F1" s="1" t="str">
         <v>Страна</v>
       </c>
       <c r="G1" s="1" t="str" xml:space="preserve">
-        <v xml:space="preserve">Откуда_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Откуда_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 покупатель</v>
       </c>
       <c r="H1" s="1" t="str" xml:space="preserve">
-        <v xml:space="preserve">Track_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Track_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 number</v>
       </c>
       <c r="I1" s="1" t="str" xml:space="preserve">
-        <v xml:space="preserve">Стоимость_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Стоимость_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 доставки</v>
       </c>
       <c r="J1" s="1" t="str" xml:space="preserve">
-        <v xml:space="preserve">Почтовая_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Почтовая_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 служба</v>
       </c>
     </row>
@@ -1615,7 +1616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -1946,4 +1947,116 @@
     <ignoredError numberStoredAsText="1" sqref="A1:G20"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="str">
+        <v>Инструмент</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <v>Регион</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <v>Количество</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <v>Дата</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="str">
+        <v>Eternal-love</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <v>ENG</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45197.057715752315</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="str">
+        <v>Aerial</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <v>ENG</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45197.059827094905</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="str">
+        <v>Infinity</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <v>ENG</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45197.060781319444</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="str">
+        <v>Infinity</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <v>UA</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <v>28.09.2023 01:36</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="str">
+        <v>Waterfall</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <v>UA</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <v>28.09.2023 01:36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="str">
+        <v>Waterfall</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <v>UA</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <v>28.09.2023 01:55</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>